<commit_message>
debuged payment test cases
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Order/auto_switching_order_test_data.xlsx
+++ b/TestData/Web_POS/Order/auto_switching_order_test_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42" count="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46" count="200">
   <si>
     <t>TC_Id</t>
   </si>
@@ -141,6 +141,18 @@
   <si>
     <t>TC_18</t>
   </si>
+  <si>
+    <t>1000 : 1</t>
+  </si>
+  <si>
+    <t>1001 : 1</t>
+  </si>
+  <si>
+    <t>1002 : 1</t>
+  </si>
+  <si>
+    <t>600 : 1</t>
+  </si>
 </sst>
 </file>
 
@@ -240,7 +252,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1125,7 +1137,7 @@
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
     </row>
-    <row r="17" spans="1:16" ht="14.25">
+    <row r="17" spans="1:16">
       <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
@@ -1145,10 +1157,10 @@
         <v>13</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>39</v>
@@ -1163,7 +1175,7 @@
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
     </row>
-    <row r="18" spans="1:16" ht="14.25">
+    <row r="18" spans="1:16">
       <c r="A18" s="1" t="s">
         <v>40</v>
       </c>
@@ -1183,10 +1195,10 @@
         <v>13</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>39</v>
@@ -1201,7 +1213,7 @@
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
     </row>
-    <row r="19" spans="1:16" ht="14.25">
+    <row r="19" spans="1:16">
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
@@ -1221,10 +1233,10 @@
         <v>13</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>39</v>

</xml_diff>